<commit_message>
Se eliminaron las carpetas RPi_Acelerometro y EsclavoAcelerometro de la carpeta Firmware y se agrego la carpeta Libreias que contiene las libreias de control del GPS y RTC DS3234 ademas del archivo de configuracion del dsPIC33EP256MC202
</commit_message>
<xml_diff>
--- a/Software/W10/Eventos.xlsx
+++ b/Software/W10/Eventos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Desktop\Milton Muñoz\Proyectos\Registro continuo\Software\W10\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Desktop\Milton Muñoz\Proyectos\Git\SistemaRegistroContinuo\SistemaRegistroContinuo\Software\W10\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -532,7 +532,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,30 +598,30 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
-        <v>1</v>
+        <v>0.6743055555555556</v>
       </c>
       <c r="C7" s="7">
-        <v>581852</v>
+        <v>5321</v>
       </c>
       <c r="D7" s="2">
         <f>ROUNDUP((C7*A3),0)</f>
-        <v>58186</v>
+        <v>533</v>
       </c>
       <c r="E7" s="8">
         <f>D7/(24*60*60)</f>
-        <v>0.67344907407407406</v>
+        <v>6.1689814814814819E-3</v>
       </c>
       <c r="F7" s="9">
         <f>((C7*0.1)/60)</f>
-        <v>969.75333333333344</v>
+        <v>8.8683333333333341</v>
       </c>
       <c r="G7" s="10">
         <f>B7+E7</f>
-        <v>1.6734490740740742</v>
+        <v>0.68047453703703709</v>
       </c>
       <c r="H7" s="10">
         <f>G7-A1</f>
-        <v>1.4651157407407409</v>
+        <v>0.47214120370370372</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -654,15 +654,15 @@
         <v>0</v>
       </c>
       <c r="C12" s="5">
-        <v>0.875</v>
+        <v>0.67569444444444438</v>
       </c>
       <c r="D12" s="15">
         <f>C12-B12</f>
-        <v>0.875</v>
+        <v>0.67569444444444438</v>
       </c>
       <c r="E12" s="15">
         <f>D12-A2</f>
-        <v>0.87361111111111112</v>
+        <v>0.67430555555555549</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>